<commit_message>
updated fig 3 to add chi2 code
</commit_message>
<xml_diff>
--- a/fig_3-s6-s7-s8-s9/custom-g-factor.xlsx
+++ b/fig_3-s6-s7-s8-s9/custom-g-factor.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/mjh/resubmission/were-anc-less-specific/fig_2ef-s6-s7-s8-s9/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harmsm/Desktop/were-anc-less-specific/fig_3-s6-s7-s8-s9/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BAA4660-F992-F341-8F30-E3137144A0A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{440D8D16-21D4-5D40-8B89-E11C59BFBA7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{7C7F0008-93D2-E34F-A220-0A22E6072269}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{7C7F0008-93D2-E34F-A220-0A22E6072269}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -420,13 +420,14 @@
   <dimension ref="A1:M130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+      <selection activeCell="E2" sqref="E2:G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="13" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.83203125" customWidth="1"/>
+    <col min="3" max="13" width="4.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -492,16 +493,13 @@
         <v>1</v>
       </c>
       <c r="E2" s="2">
-        <f>1.005</f>
-        <v>1.0049999999999999</v>
+        <v>1.0029999999999999</v>
       </c>
       <c r="F2" s="2">
-        <f t="shared" ref="F2:G9" si="1">1.005</f>
-        <v>1.0049999999999999</v>
+        <v>1.0029999999999999</v>
       </c>
       <c r="G2" s="2">
-        <f t="shared" si="1"/>
-        <v>1.0049999999999999</v>
+        <v>1.0029999999999999</v>
       </c>
       <c r="H2" s="2">
         <v>1</v>
@@ -513,16 +511,13 @@
         <v>1</v>
       </c>
       <c r="K2" s="2">
-        <f t="shared" ref="K2:M9" si="2">1.005</f>
-        <v>1.0049999999999999</v>
+        <v>1.004</v>
       </c>
       <c r="L2" s="2">
-        <f t="shared" si="2"/>
-        <v>1.0049999999999999</v>
+        <v>1.004</v>
       </c>
       <c r="M2" s="2">
-        <f t="shared" si="2"/>
-        <v>1.0049999999999999</v>
+        <v>1.004</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
@@ -539,16 +534,13 @@
         <v>1</v>
       </c>
       <c r="E3" s="2">
-        <f t="shared" ref="E3:E9" si="3">1.005</f>
-        <v>1.0049999999999999</v>
+        <v>1.0029999999999999</v>
       </c>
       <c r="F3" s="2">
-        <f t="shared" si="1"/>
-        <v>1.0049999999999999</v>
+        <v>1.0029999999999999</v>
       </c>
       <c r="G3" s="2">
-        <f t="shared" si="1"/>
-        <v>1.0049999999999999</v>
+        <v>1.0029999999999999</v>
       </c>
       <c r="H3" s="2">
         <v>1</v>
@@ -560,16 +552,13 @@
         <v>1</v>
       </c>
       <c r="K3" s="2">
-        <f t="shared" si="2"/>
-        <v>1.0049999999999999</v>
+        <v>1.004</v>
       </c>
       <c r="L3" s="2">
-        <f t="shared" si="2"/>
-        <v>1.0049999999999999</v>
+        <v>1.004</v>
       </c>
       <c r="M3" s="2">
-        <f t="shared" si="2"/>
-        <v>1.0049999999999999</v>
+        <v>1.004</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
@@ -586,16 +575,13 @@
         <v>1</v>
       </c>
       <c r="E4" s="2">
-        <f t="shared" si="3"/>
-        <v>1.0049999999999999</v>
+        <v>1.0029999999999999</v>
       </c>
       <c r="F4" s="2">
-        <f t="shared" si="1"/>
-        <v>1.0049999999999999</v>
+        <v>1.0029999999999999</v>
       </c>
       <c r="G4" s="2">
-        <f t="shared" si="1"/>
-        <v>1.0049999999999999</v>
+        <v>1.0029999999999999</v>
       </c>
       <c r="H4" s="2">
         <v>1</v>
@@ -607,16 +593,13 @@
         <v>1</v>
       </c>
       <c r="K4" s="2">
-        <f t="shared" si="2"/>
-        <v>1.0049999999999999</v>
+        <v>1.004</v>
       </c>
       <c r="L4" s="2">
-        <f t="shared" si="2"/>
-        <v>1.0049999999999999</v>
+        <v>1.004</v>
       </c>
       <c r="M4" s="2">
-        <f t="shared" si="2"/>
-        <v>1.0049999999999999</v>
+        <v>1.004</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
@@ -633,16 +616,13 @@
         <v>1</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" si="3"/>
-        <v>1.0049999999999999</v>
+        <v>1.0029999999999999</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" si="1"/>
-        <v>1.0049999999999999</v>
+        <v>1.0029999999999999</v>
       </c>
       <c r="G5" s="2">
-        <f t="shared" si="1"/>
-        <v>1.0049999999999999</v>
+        <v>1.0029999999999999</v>
       </c>
       <c r="H5" s="2">
         <v>1</v>
@@ -654,16 +634,13 @@
         <v>1</v>
       </c>
       <c r="K5" s="2">
-        <f t="shared" si="2"/>
-        <v>1.0049999999999999</v>
+        <v>1.004</v>
       </c>
       <c r="L5" s="2">
-        <f t="shared" si="2"/>
-        <v>1.0049999999999999</v>
+        <v>1.004</v>
       </c>
       <c r="M5" s="2">
-        <f t="shared" si="2"/>
-        <v>1.0049999999999999</v>
+        <v>1.004</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
@@ -680,16 +657,13 @@
         <v>1</v>
       </c>
       <c r="E6" s="2">
-        <f t="shared" si="3"/>
-        <v>1.0049999999999999</v>
+        <v>1.0029999999999999</v>
       </c>
       <c r="F6" s="2">
-        <f t="shared" si="1"/>
-        <v>1.0049999999999999</v>
+        <v>1.0029999999999999</v>
       </c>
       <c r="G6" s="2">
-        <f t="shared" si="1"/>
-        <v>1.0049999999999999</v>
+        <v>1.0029999999999999</v>
       </c>
       <c r="H6" s="2">
         <v>1</v>
@@ -701,16 +675,13 @@
         <v>1</v>
       </c>
       <c r="K6" s="2">
-        <f t="shared" si="2"/>
-        <v>1.0049999999999999</v>
+        <v>1.004</v>
       </c>
       <c r="L6" s="2">
-        <f t="shared" si="2"/>
-        <v>1.0049999999999999</v>
+        <v>1.004</v>
       </c>
       <c r="M6" s="2">
-        <f t="shared" si="2"/>
-        <v>1.0049999999999999</v>
+        <v>1.004</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -727,16 +698,13 @@
         <v>1</v>
       </c>
       <c r="E7" s="2">
-        <f t="shared" si="3"/>
-        <v>1.0049999999999999</v>
+        <v>1.0029999999999999</v>
       </c>
       <c r="F7" s="2">
-        <f t="shared" si="1"/>
-        <v>1.0049999999999999</v>
+        <v>1.0029999999999999</v>
       </c>
       <c r="G7" s="2">
-        <f t="shared" si="1"/>
-        <v>1.0049999999999999</v>
+        <v>1.0029999999999999</v>
       </c>
       <c r="H7" s="2">
         <v>1</v>
@@ -748,16 +716,13 @@
         <v>1</v>
       </c>
       <c r="K7" s="2">
-        <f t="shared" si="2"/>
-        <v>1.0049999999999999</v>
+        <v>1.004</v>
       </c>
       <c r="L7" s="2">
-        <f t="shared" si="2"/>
-        <v>1.0049999999999999</v>
+        <v>1.004</v>
       </c>
       <c r="M7" s="2">
-        <f t="shared" si="2"/>
-        <v>1.0049999999999999</v>
+        <v>1.004</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -774,16 +739,13 @@
         <v>1</v>
       </c>
       <c r="E8" s="2">
-        <f t="shared" si="3"/>
-        <v>1.0049999999999999</v>
+        <v>1.0029999999999999</v>
       </c>
       <c r="F8" s="2">
-        <f t="shared" si="1"/>
-        <v>1.0049999999999999</v>
+        <v>1.0029999999999999</v>
       </c>
       <c r="G8" s="2">
-        <f t="shared" si="1"/>
-        <v>1.0049999999999999</v>
+        <v>1.0029999999999999</v>
       </c>
       <c r="H8" s="2">
         <v>1</v>
@@ -795,16 +757,13 @@
         <v>1</v>
       </c>
       <c r="K8" s="2">
-        <f t="shared" si="2"/>
-        <v>1.0049999999999999</v>
+        <v>1.004</v>
       </c>
       <c r="L8" s="2">
-        <f t="shared" si="2"/>
-        <v>1.0049999999999999</v>
+        <v>1.004</v>
       </c>
       <c r="M8" s="2">
-        <f t="shared" si="2"/>
-        <v>1.0049999999999999</v>
+        <v>1.004</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -821,16 +780,13 @@
         <v>1</v>
       </c>
       <c r="E9" s="2">
-        <f t="shared" si="3"/>
-        <v>1.0049999999999999</v>
+        <v>1.0029999999999999</v>
       </c>
       <c r="F9" s="2">
-        <f t="shared" si="1"/>
-        <v>1.0049999999999999</v>
+        <v>1.0029999999999999</v>
       </c>
       <c r="G9" s="2">
-        <f t="shared" si="1"/>
-        <v>1.0049999999999999</v>
+        <v>1.0029999999999999</v>
       </c>
       <c r="H9" s="2">
         <v>1</v>
@@ -842,16 +798,13 @@
         <v>1</v>
       </c>
       <c r="K9" s="2">
-        <f t="shared" si="2"/>
-        <v>1.0049999999999999</v>
+        <v>1.004</v>
       </c>
       <c r="L9" s="2">
-        <f t="shared" si="2"/>
-        <v>1.0049999999999999</v>
+        <v>1.004</v>
       </c>
       <c r="M9" s="2">
-        <f t="shared" si="2"/>
-        <v>1.0049999999999999</v>
+        <v>1.004</v>
       </c>
     </row>
     <row r="130" spans="11:11" x14ac:dyDescent="0.2">

</xml_diff>